<commit_message>
all scripts and figures ready for publication
</commit_message>
<xml_diff>
--- a/DATA/squid_all_plot_data.xlsx
+++ b/DATA/squid_all_plot_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/Squid/Squid/CODE/Squid/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285CBE75-5DAD-6E4B-A7D3-583C1ECAC928}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B0CA7E-2A71-B84C-9FA2-8916AC549DBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{BA4F5C29-8DDB-0E4B-86A5-B76B9BC824F8}"/>
   </bookViews>
@@ -64,7 +64,93 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{939FB306-6EA2-2F4A-A3BF-DC2A8791D8B5}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{939FB306-6EA2-2F4A-A3BF-DC2A8791D8B5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">prices for fishers in Guaymas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">2001-2016:Datamares (data_Elsler.xlsx
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve"> &amp; tableau: data_ElslerAllSpecies_CPIMXN.tbw) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{D1DA3336-34EB-894D-85EE-0B0878094F79}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">prices for fishers in all other offices
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">2001-2016:Datamares (data_Elsler.xlsx
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve"> &amp; tableau: data_ElslerAllSpecies_CPIMXN.tbw) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{9311F6EC-ABEC-0648-A103-C0A47D3E4F07}">
       <text>
         <r>
           <rPr>
@@ -74,7 +160,7 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t xml:space="preserve">prices for fishers in Guaymas 
+          <t xml:space="preserve">prices for fishers in Santa Rosalia 
 </t>
         </r>
         <r>
@@ -108,8 +194,181 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D1DA3336-34EB-894D-85EE-0B0878094F79}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{41CFAB6F-A7BF-CE45-AD3A-7F30710D3A41}">
       <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1991-2014: proportion of migrated squid Tim data (AnuarioSquid.xlsx)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2014-2016: DM (LandingsLocationDM.xlsx)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B01AA821-3495-6446-95AA-A9C8DDDDA798}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1996-2017: Mantle length timeseries from Gilly data 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">(source: ML_composite
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">processed in: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MLtimeSeries.xlsx)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{4A7DAD3A-E20E-CE49-A350-4863D2A98BD0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Sea surface temperature anomaly from Greg 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">(source: SST_anomaly.csv
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">processed in:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SST_anom_lge.xlsx)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{F09E0559-A297-8345-B1A1-C7BBB0436B59}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sum of all datamares catch data</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{984F7EF1-999B-A948-9646-B6B4200153EE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">catch in Guaymas 
+</t>
+        </r>
         <r>
           <rPr>
             <sz val="11"/>
@@ -117,7 +376,7 @@
             <rFont val="Calibri"/>
             <family val="34"/>
           </rPr>
-          <t xml:space="preserve">prices for fishers in all other offices
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -127,6 +386,39 @@
             <rFont val="Calibri"/>
             <family val="34"/>
           </rPr>
+          <t xml:space="preserve">2001-2016:Datamares (data_Elsler.xlsx
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve"> &amp; tableau: data_ElslerAllSpecies_CPIMXN.tbw) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{95FADC58-427F-FF41-83B8-59846C14F211}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">catch in all other offices
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
           <t xml:space="preserve">
 </t>
         </r>
@@ -151,7 +443,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9311F6EC-ABEC-0648-A103-C0A47D3E4F07}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{12540892-B069-2044-BAC8-4A95BFD85CAE}">
       <text>
         <r>
           <rPr>
@@ -159,9 +451,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">prices for fishers in Santa Rosalia 
+          </rPr>
+          <t xml:space="preserve">catch in Santa Rosalia 
 </t>
         </r>
         <r>
@@ -192,309 +483,6 @@
             <family val="34"/>
           </rPr>
           <t xml:space="preserve"> &amp; tableau: data_ElslerAllSpecies_CPIMXN.tbw) </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{41CFAB6F-A7BF-CE45-AD3A-7F30710D3A41}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">1991-2014: proportion of migrated squid Tim data (AnuarioSquid.xlsx)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2014-2016: DM (LandingsLocationDM.xlsx)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B01AA821-3495-6446-95AA-A9C8DDDDA798}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">1996-2017: Mantle length timeseries from Gilly data </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">(source: ML_composite
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">processed in: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MLtimeSeries.xlsx)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{4A7DAD3A-E20E-CE49-A350-4863D2A98BD0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Sea surface temperature anomaly from Greg 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">(source: SST_anomaly.csv
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">processed in:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>SST_anom_lge.xlsx)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{984F7EF1-999B-A948-9646-B6B4200153EE}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">catch in Guaymas 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">2001-2016:Datamares (data_Elsler.xlsx
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> &amp; tableau: data_ElslerAllSpecies_CPIMXN.tbw) </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{95FADC58-427F-FF41-83B8-59846C14F211}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">catch in all other offices
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">2001-2016:Datamares (data_Elsler.xlsx
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> &amp; tableau: data_ElslerAllSpecies_CPIMXN.tbw) </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{12540892-B069-2044-BAC8-4A95BFD85CAE}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">catch in Santa Rosalia 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">2001-2016:Datamares (data_Elsler.xlsx
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> &amp; tableau: data_ElslerAllSpecies_CPIMXN.tbw) </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{F09E0559-A297-8345-B1A1-C7BBB0436B59}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sum of all datamares catch data</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
         </r>
       </text>
     </comment>
@@ -503,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="214">
   <si>
     <t>year</t>
   </si>
@@ -511,9 +499,6 @@
     <t>ML</t>
   </si>
   <si>
-    <t>y_S</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -523,9 +508,6 @@
     <t>pf_GY</t>
   </si>
   <si>
-    <t>pf_rm</t>
-  </si>
-  <si>
     <t>pf_SR</t>
   </si>
   <si>
@@ -556,9 +538,6 @@
     <t>C_SR</t>
   </si>
   <si>
-    <t>C_AL</t>
-  </si>
-  <si>
     <t>1.815573913</t>
   </si>
   <si>
@@ -1088,16 +1067,84 @@
   </si>
   <si>
     <t>1137.907</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>6000.0</t>
+  </si>
+  <si>
+    <t>pf_RM</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>pf_ALL</t>
+  </si>
+  <si>
+    <t>C_ALL</t>
+  </si>
+  <si>
+    <t>2985.12859623229</t>
+  </si>
+  <si>
+    <t>3262.06476645813</t>
+  </si>
+  <si>
+    <t>2554.71802625929</t>
+  </si>
+  <si>
+    <t>3086.20899305451</t>
+  </si>
+  <si>
+    <t>3202.37797964527</t>
+  </si>
+  <si>
+    <t>3015.74698011062</t>
+  </si>
+  <si>
+    <t>3611.77160422671</t>
+  </si>
+  <si>
+    <t>2559.51510387858</t>
+  </si>
+  <si>
+    <t>2592.78743533779</t>
+  </si>
+  <si>
+    <t>3780.76439575705</t>
+  </si>
+  <si>
+    <t>5529.2149917346</t>
+  </si>
+  <si>
+    <t>5346.36453363053</t>
+  </si>
+  <si>
+    <t>7833.79783062461</t>
+  </si>
+  <si>
+    <t>9238.32842300856</t>
+  </si>
+  <si>
+    <t>10147.7843515686</t>
+  </si>
+  <si>
+    <t>15438.0198734057</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1175,7 +1222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1184,6 +1231,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1498,843 +1547,911 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C701C87-3C98-B146-B861-6449297CC094}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1991</v>
       </c>
       <c r="B2">
         <v>5486</v>
       </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G2" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1992</v>
       </c>
       <c r="B3">
         <v>8549</v>
       </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G3" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1993</v>
       </c>
       <c r="B4">
         <v>3043</v>
       </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G4" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1994</v>
       </c>
       <c r="B5">
         <v>1800</v>
       </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G5" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1995</v>
       </c>
       <c r="B6">
         <v>39567</v>
       </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G6" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1996</v>
       </c>
       <c r="B7">
         <v>107967</v>
       </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G7" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1997</v>
       </c>
       <c r="B8">
         <v>120877</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1998</v>
       </c>
       <c r="B9">
         <v>26611</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1999</v>
       </c>
       <c r="B10">
         <v>57985</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2000</v>
       </c>
       <c r="B11">
         <v>56153</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2001</v>
       </c>
       <c r="B12">
         <v>73741</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="J12" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="M12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2002</v>
       </c>
       <c r="B13">
         <v>115896</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="J13" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="M13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2003</v>
       </c>
       <c r="B14">
         <v>97332</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="J14" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="M14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2004</v>
       </c>
       <c r="B15">
         <v>87228</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="J15" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="M15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2005</v>
       </c>
       <c r="B16">
         <v>53437</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="J16" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="M16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2006</v>
       </c>
       <c r="B17">
         <v>65611</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="J17" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="M17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2007</v>
       </c>
       <c r="B18">
         <v>57476</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="J18" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="M18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2008</v>
       </c>
       <c r="B19">
         <v>84437</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="J19" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="M19" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2009</v>
       </c>
       <c r="B20">
         <v>57894</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="J20" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="M20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2010</v>
       </c>
       <c r="B21">
         <v>42893</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="H21" s="2">
+        <v>46</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="J21" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="L21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G21" s="2">
-        <v>46</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="M21" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2011</v>
       </c>
       <c r="B22">
         <v>34844</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="J22" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="M22" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2012</v>
       </c>
       <c r="B23">
         <v>23157</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="J23" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="M23" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2013</v>
       </c>
       <c r="B24">
         <v>9014</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="H24" s="2">
+        <v>45</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="J24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="L24" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G24" s="2">
-        <v>45</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="M24" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2014</v>
       </c>
       <c r="B25">
         <v>36729</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="J25" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="M25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2015</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="J26" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="L26" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="M26" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2016</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="J27" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="L27" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2017</v>
       </c>
-      <c r="D28" s="3">
-        <v>6000</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="I28" s="2"/>
+      <c r="E28" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="J28" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F29" s="3"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F30" s="3"/>
-      <c r="H30" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G29" s="3"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="3"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2354,27 +2471,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>2001</v>
@@ -2394,7 +2511,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2002</v>
@@ -2414,7 +2531,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>2003</v>
@@ -2434,7 +2551,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2004</v>
@@ -2454,7 +2571,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>2005</v>
@@ -2474,7 +2591,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>2006</v>
@@ -2494,7 +2611,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2007</v>
@@ -2514,7 +2631,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2008</v>
@@ -2534,7 +2651,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>2009</v>
@@ -2554,7 +2671,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>2010</v>
@@ -2574,7 +2691,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>2011</v>
@@ -2594,7 +2711,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>2012</v>
@@ -2614,7 +2731,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>2013</v>
@@ -2634,7 +2751,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>2014</v>
@@ -2654,7 +2771,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>2015</v>
@@ -2674,7 +2791,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>2016</v>
@@ -2694,7 +2811,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>2001</v>
@@ -2711,7 +2828,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>2002</v>
@@ -2725,7 +2842,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20">
         <v>2003</v>
@@ -2739,7 +2856,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>2004</v>
@@ -2753,7 +2870,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>2005</v>
@@ -2767,7 +2884,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>2006</v>
@@ -2781,7 +2898,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24">
         <v>2007</v>
@@ -2795,7 +2912,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>2008</v>
@@ -2809,7 +2926,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>2009</v>
@@ -2823,7 +2940,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>2010</v>
@@ -2837,7 +2954,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>2011</v>
@@ -2851,7 +2968,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>2012</v>
@@ -2865,7 +2982,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>2013</v>
@@ -2879,7 +2996,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>2014</v>
@@ -2893,7 +3010,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>2015</v>
@@ -2907,7 +3024,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>2016</v>
@@ -2921,7 +3038,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34">
         <v>2017</v>
@@ -2935,7 +3052,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>2001</v>
@@ -2949,7 +3066,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>2002</v>
@@ -2963,7 +3080,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>2003</v>
@@ -2977,7 +3094,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B38">
         <v>2004</v>
@@ -2991,7 +3108,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <v>2005</v>
@@ -3005,7 +3122,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40">
         <v>2006</v>
@@ -3019,7 +3136,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>2007</v>
@@ -3033,7 +3150,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42">
         <v>2008</v>
@@ -3047,7 +3164,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>2009</v>
@@ -3061,7 +3178,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44">
         <v>2010</v>
@@ -3075,7 +3192,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B45">
         <v>2011</v>
@@ -3089,7 +3206,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B46">
         <v>2012</v>
@@ -3103,7 +3220,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>2013</v>
@@ -3117,7 +3234,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>2014</v>
@@ -3131,7 +3248,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B49">
         <v>2015</v>
@@ -3145,7 +3262,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50">
         <v>2016</v>

</xml_diff>

<commit_message>
move old files to March folder
</commit_message>
<xml_diff>
--- a/DATA/squid_all_plot_data.xlsx
+++ b/DATA/squid_all_plot_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/Squid/Squid/CODE/Squid/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B0CA7E-2A71-B84C-9FA2-8916AC549DBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD663137-627D-8C4F-BF97-008E7F5FDD94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{BA4F5C29-8DDB-0E4B-86A5-B76B9BC824F8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BA4F5C29-8DDB-0E4B-86A5-B76B9BC824F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">prices for fishers in Santa Rosalia 
 </t>
@@ -227,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B01AA821-3495-6446-95AA-A9C8DDDDA798}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{B01AA821-3495-6446-95AA-A9C8DDDDA798}">
       <text>
         <r>
           <rPr>
@@ -280,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{4A7DAD3A-E20E-CE49-A350-4863D2A98BD0}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{4A7DAD3A-E20E-CE49-A350-4863D2A98BD0}">
       <text>
         <r>
           <rPr>
@@ -333,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{F09E0559-A297-8345-B1A1-C7BBB0436B59}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{F09E0559-A297-8345-B1A1-C7BBB0436B59}">
       <text>
         <r>
           <rPr>
@@ -357,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{984F7EF1-999B-A948-9646-B6B4200153EE}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{984F7EF1-999B-A948-9646-B6B4200153EE}">
       <text>
         <r>
           <rPr>
@@ -400,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{95FADC58-427F-FF41-83B8-59846C14F211}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{95FADC58-427F-FF41-83B8-59846C14F211}">
       <text>
         <r>
           <rPr>
@@ -443,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{12540892-B069-2044-BAC8-4A95BFD85CAE}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{12540892-B069-2044-BAC8-4A95BFD85CAE}">
       <text>
         <r>
           <rPr>
@@ -491,7 +490,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="194">
   <si>
     <t>year</t>
   </si>
@@ -556,36 +555,24 @@
     <t>0.026812565</t>
   </si>
   <si>
-    <t>0.073496</t>
-  </si>
-  <si>
     <t>68.7</t>
   </si>
   <si>
     <t>-0.557240247</t>
   </si>
   <si>
-    <t>0.676825</t>
-  </si>
-  <si>
     <t>28.7</t>
   </si>
   <si>
     <t>3.518298951</t>
   </si>
   <si>
-    <t>0.000655</t>
-  </si>
-  <si>
     <t>46.8</t>
   </si>
   <si>
     <t>-1.07852608</t>
   </si>
   <si>
-    <t>0.112443</t>
-  </si>
-  <si>
     <t>35.8</t>
   </si>
   <si>
@@ -601,9 +588,6 @@
     <t>2572.852269445</t>
   </si>
   <si>
-    <t>0.00038</t>
-  </si>
-  <si>
     <t>50.4</t>
   </si>
   <si>
@@ -628,9 +612,6 @@
     <t>2910.428058834</t>
   </si>
   <si>
-    <t>0.00252</t>
-  </si>
-  <si>
     <t>65.6</t>
   </si>
   <si>
@@ -655,9 +636,6 @@
     <t>2313.459647507</t>
   </si>
   <si>
-    <t>0.000092</t>
-  </si>
-  <si>
     <t>56.4</t>
   </si>
   <si>
@@ -682,9 +660,6 @@
     <t>2802.089454061</t>
   </si>
   <si>
-    <t>0.00219</t>
-  </si>
-  <si>
     <t>64.8</t>
   </si>
   <si>
@@ -709,9 +684,6 @@
     <t>2685.455833096</t>
   </si>
   <si>
-    <t>0.088721</t>
-  </si>
-  <si>
     <t>59.6</t>
   </si>
   <si>
@@ -736,9 +708,6 @@
     <t>2976.704799272</t>
   </si>
   <si>
-    <t>0.033866</t>
-  </si>
-  <si>
     <t>62.9</t>
   </si>
   <si>
@@ -763,9 +732,6 @@
     <t>4064.103784431</t>
   </si>
   <si>
-    <t>0.04501</t>
-  </si>
-  <si>
     <t>66.7</t>
   </si>
   <si>
@@ -790,9 +756,6 @@
     <t>2358.870121859</t>
   </si>
   <si>
-    <t>0.084169</t>
-  </si>
-  <si>
     <t>69.2</t>
   </si>
   <si>
@@ -817,9 +780,6 @@
     <t>2390.402628025</t>
   </si>
   <si>
-    <t>0.071389</t>
-  </si>
-  <si>
     <t>30.8</t>
   </si>
   <si>
@@ -844,9 +804,6 @@
     <t>3834.284563766</t>
   </si>
   <si>
-    <t>0.584291</t>
-  </si>
-  <si>
     <t>0.985399409</t>
   </si>
   <si>
@@ -868,9 +825,6 @@
     <t>5631.934531874</t>
   </si>
   <si>
-    <t>0.405407</t>
-  </si>
-  <si>
     <t>32.5</t>
   </si>
   <si>
@@ -895,9 +849,6 @@
     <t>5709.578480761</t>
   </si>
   <si>
-    <t>0.441378</t>
-  </si>
-  <si>
     <t>36.4</t>
   </si>
   <si>
@@ -922,9 +873,6 @@
     <t>4643.591460062</t>
   </si>
   <si>
-    <t>0.414799</t>
-  </si>
-  <si>
     <t>-1.179877307</t>
   </si>
   <si>
@@ -946,9 +894,6 @@
     <t>4393.560097463</t>
   </si>
   <si>
-    <t>0.014539</t>
-  </si>
-  <si>
     <t>46.1</t>
   </si>
   <si>
@@ -973,9 +918,6 @@
     <t>5729.434141228</t>
   </si>
   <si>
-    <t>0.817414156917821</t>
-  </si>
-  <si>
     <t>20.1</t>
   </si>
   <si>
@@ -1000,9 +942,6 @@
     <t>4139.072847682</t>
   </si>
   <si>
-    <t>0.927960720867347</t>
-  </si>
-  <si>
     <t>18.1</t>
   </si>
   <si>
@@ -1069,9 +1008,6 @@
     <t>1137.907</t>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
     <t>6000.0</t>
   </si>
   <si>
@@ -1133,20 +1069,21 @@
   </si>
   <si>
     <t>15438.0198734057</t>
+  </si>
+  <si>
+    <t>M_new</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000000"/>
-    <numFmt numFmtId="168" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1176,13 +1113,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1222,7 +1152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1231,8 +1161,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1547,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C701C87-3C98-B146-B861-6449297CC094}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1560,13 +1488,14 @@
     <col min="3" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1574,207 +1503,250 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>197</v>
-      </c>
       <c r="K1" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1991</v>
       </c>
       <c r="B2">
         <v>5486</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1992</v>
       </c>
       <c r="B3">
         <v>8549</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1993</v>
       </c>
       <c r="B4">
         <v>3043</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
         <v>1</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1994</v>
       </c>
       <c r="B5">
         <v>1800</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1995</v>
       </c>
       <c r="B6">
         <v>39567</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1996</v>
       </c>
       <c r="B7">
         <v>107967</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1997</v>
       </c>
       <c r="B8">
         <v>120877</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="6">
+        <v>7.3496000000000006E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>6.8464330576983798E-2</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1998</v>
       </c>
       <c r="B9">
         <v>26611</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="6">
+        <v>0.67682500000000001</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.40363497826184402</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1999</v>
       </c>
       <c r="B10">
         <v>57985</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G10" s="6">
+        <v>6.5499999999999998E-4</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6.5491270702997104E-4</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2000</v>
       </c>
       <c r="B11">
         <v>56153</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G11" s="6">
+        <v>0.112443</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.101077368850753</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2001</v>
       </c>
@@ -1782,40 +1754,44 @@
         <v>73741</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="6">
+        <v>3.8000000000000002E-4</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.98536072366519E-2</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="K12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="M12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="N12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -1823,40 +1799,44 @@
         <v>115896</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2.5200000000000001E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4.6249194900379299E-2</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="M13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="N13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2003</v>
       </c>
@@ -1864,40 +1844,44 @@
         <v>97332</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="6">
+        <v>9.2E-5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.9584892735141399E-2</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="N14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2004</v>
       </c>
@@ -1905,40 +1889,44 @@
         <v>87228</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2.1900000000000001E-3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>4.5536408800865999E-2</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2005</v>
       </c>
@@ -1946,40 +1934,44 @@
         <v>53437</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>180</v>
+        <v>63</v>
+      </c>
+      <c r="G16" s="6">
+        <v>8.8720999999999994E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.116473106537236</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2006</v>
       </c>
@@ -1987,40 +1979,44 @@
         <v>65611</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>181</v>
+        <v>71</v>
+      </c>
+      <c r="G17" s="6">
+        <v>3.3866E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5.4764327928591497E-2</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2007</v>
       </c>
@@ -2028,40 +2024,44 @@
         <v>57476</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>182</v>
+        <v>79</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4.5010000000000001E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7.8384788044696396E-2</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2008</v>
       </c>
@@ -2069,40 +2069,44 @@
         <v>84437</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>183</v>
+        <v>87</v>
+      </c>
+      <c r="G19" s="6">
+        <v>8.4168999999999994E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>8.6864051049876503E-2</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2009</v>
       </c>
@@ -2110,40 +2114,44 @@
         <v>57894</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>184</v>
+        <v>95</v>
+      </c>
+      <c r="G20" s="6">
+        <v>7.1388999999999994E-2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>9.5626055261100198E-2</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2010</v>
       </c>
@@ -2151,40 +2159,44 @@
         <v>42893</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>117</v>
+        <v>103</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.584291</v>
       </c>
       <c r="H21" s="2">
+        <v>0.442268155099306</v>
+      </c>
+      <c r="I21" s="2">
         <v>46</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>185</v>
+      <c r="J21" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2011</v>
       </c>
@@ -2192,40 +2204,44 @@
         <v>34844</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>186</v>
+        <v>110</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.40540700000000002</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.34388322311435199</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2012</v>
       </c>
@@ -2233,40 +2249,44 @@
         <v>23157</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>187</v>
+        <v>118</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.44137799999999999</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.402384408016426</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2013</v>
       </c>
@@ -2274,40 +2294,44 @@
         <v>9014</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.41479899999999997</v>
       </c>
       <c r="H24" s="2">
+        <v>0.63046586349497502</v>
+      </c>
+      <c r="I24" s="2">
         <v>45</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>188</v>
+      <c r="J24" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2014</v>
       </c>
@@ -2315,143 +2339,161 @@
         <v>36729</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>189</v>
+        <v>133</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1.4539E-2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.13546306769734501</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2015</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>190</v>
+        <v>141</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.81741415691782104</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.53818259593437601</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2016</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>191</v>
+        <v>149</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.92796072086734704</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.40366993504326898</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>171</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2017</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="N28" s="2"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="3"/>
-      <c r="K29" s="5"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="J30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final plots and scripts
</commit_message>
<xml_diff>
--- a/DATA/squid_all_plot_data.xlsx
+++ b/DATA/squid_all_plot_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/Squid/Squid/CODE/Squid/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD663137-627D-8C4F-BF97-008E7F5FDD94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CC7478-19B4-244C-A20B-46FC58AAFC0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BA4F5C29-8DDB-0E4B-86A5-B76B9BC824F8}"/>
   </bookViews>
@@ -223,6 +223,20 @@
             <family val="2"/>
           </rPr>
           <t>2014-2016: DM (LandingsLocationDM.xlsx)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{2570C971-7783-2A45-8284-9FFDCD581C73}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Old file M</t>
         </r>
       </text>
     </comment>
@@ -1478,7 +1492,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
four scripts all plots- corrected graphics
</commit_message>
<xml_diff>
--- a/DATA/squid_all_plot_data.xlsx
+++ b/DATA/squid_all_plot_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/Squid/Squid/CODE/Squid/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CC7478-19B4-244C-A20B-46FC58AAFC0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AD6303-2C27-0142-BDC7-672F019CFAC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BA4F5C29-8DDB-0E4B-86A5-B76B9BC824F8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{BA4F5C29-8DDB-0E4B-86A5-B76B9BC824F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1492,7 +1492,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I2" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1560,15 +1560,8 @@
       <c r="B2">
         <v>5486</v>
       </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="2"/>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1578,15 +1571,8 @@
       <c r="B3">
         <v>8549</v>
       </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="2"/>
       <c r="J3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1599,15 +1585,8 @@
       <c r="B4">
         <v>3043</v>
       </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="2"/>
       <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1620,15 +1599,8 @@
       <c r="B5">
         <v>1800</v>
       </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="2"/>
       <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1641,15 +1613,8 @@
       <c r="B6">
         <v>39567</v>
       </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="2"/>
       <c r="J6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1662,12 +1627,8 @@
       <c r="B7">
         <v>107967</v>
       </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
change colors of ML,M plotting
</commit_message>
<xml_diff>
--- a/DATA/squid_all_plot_data.xlsx
+++ b/DATA/squid_all_plot_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauraelsler/Dropbox/PhD/Resources/Squid/Squid/CODE/Squid/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AD6303-2C27-0142-BDC7-672F019CFAC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC11E54-73C1-2E45-932E-231B8F2E7E42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{BA4F5C29-8DDB-0E4B-86A5-B76B9BC824F8}"/>
   </bookViews>
@@ -1492,7 +1492,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1560,8 +1560,15 @@
       <c r="B2">
         <v>5486</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1571,8 +1578,15 @@
       <c r="B3">
         <v>8549</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
       <c r="J3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1585,8 +1599,15 @@
       <c r="B4">
         <v>3043</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
       <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1599,8 +1620,15 @@
       <c r="B5">
         <v>1800</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
       <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1613,8 +1641,15 @@
       <c r="B6">
         <v>39567</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
       <c r="J6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1627,8 +1662,12 @@
       <c r="B7">
         <v>107967</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>